<commit_message>
I think Im done with this calculator
</commit_message>
<xml_diff>
--- a/clay_thermo_calculator_berth3.xlsx
+++ b/clay_thermo_calculator_berth3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="19200" windowHeight="6980" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="19200" windowHeight="6975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="6" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="table 3" sheetId="2" r:id="rId6"/>
     <sheet name="table 4" sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -1035,7 +1035,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1323,7 +1323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1356,26 +1356,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1408,23 +1391,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1604,24 +1570,24 @@
   <sheetPr published="0"/>
   <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" customWidth="1"/>
-    <col min="17" max="17" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>127</v>
       </c>
@@ -1629,7 +1595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" ht="19.5" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>30</v>
       </c>
@@ -1673,7 +1639,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1729,7 +1695,7 @@
         <v>-3451.9633765265585</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1771,7 +1737,7 @@
         <v>-3435.8933765265583</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -1813,7 +1779,7 @@
       </c>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -1857,7 +1823,7 @@
       </c>
       <c r="R6" s="7"/>
     </row>
-    <row r="7" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -1898,7 +1864,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -1939,7 +1905,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1980,7 +1946,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -2021,7 +1987,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>5</v>
@@ -2062,7 +2028,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
@@ -2103,7 +2069,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
@@ -2143,7 +2109,7 @@
       </c>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -2184,7 +2150,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -2225,7 +2191,7 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
@@ -2262,7 +2228,7 @@
         <v>4.1840000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
@@ -2302,7 +2268,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
@@ -2343,7 +2309,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>13</v>
@@ -2383,7 +2349,7 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>14</v>
@@ -2421,7 +2387,7 @@
       </c>
       <c r="R20" s="3"/>
     </row>
-    <row r="21" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>116</v>
       </c>
@@ -2442,7 +2408,7 @@
       </c>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -2483,7 +2449,7 @@
       </c>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>16</v>
@@ -2524,7 +2490,7 @@
       </c>
       <c r="R23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>17</v>
@@ -2566,7 +2532,7 @@
       </c>
       <c r="R24" s="3"/>
     </row>
-    <row r="25" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>18</v>
@@ -2607,7 +2573,7 @@
       </c>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>3</v>
@@ -2624,7 +2590,7 @@
         <v>0.5</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G23:G31" si="6">IF(D26,F26*D26,0)</f>
+        <f t="shared" ref="G26:G31" si="6">IF(D26,F26*D26,0)</f>
         <v>0</v>
       </c>
       <c r="H26">
@@ -2647,7 +2613,7 @@
       </c>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>4</v>
@@ -2687,7 +2653,7 @@
       </c>
       <c r="R27" s="3"/>
     </row>
-    <row r="28" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -2727,7 +2693,7 @@
       </c>
       <c r="R28" s="3"/>
     </row>
-    <row r="29" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>9</v>
@@ -2767,7 +2733,7 @@
       </c>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>19</v>
@@ -2807,7 +2773,7 @@
       </c>
       <c r="R30" s="3"/>
     </row>
-    <row r="31" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>36</v>
@@ -2846,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>116</v>
       </c>
@@ -2862,7 +2828,7 @@
         <v>-242.82459459459457</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -2902,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>16</v>
@@ -2942,7 +2908,7 @@
         <v>-424.38240000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>17</v>
@@ -2983,7 +2949,7 @@
         <v>-184.327</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>18</v>
@@ -3023,7 +2989,7 @@
         <v>-90.885300000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>3</v>
@@ -3062,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>4</v>
@@ -3101,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
@@ -3140,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
         <v>9</v>
@@ -3179,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>19</v>
@@ -3218,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
         <v>36</v>
@@ -3257,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>116</v>
       </c>
@@ -3277,7 +3243,7 @@
         <v>-248.2205193279766</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>126</v>
       </c>
@@ -3317,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
         <v>16</v>
@@ -3355,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>17</v>
@@ -3393,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>18</v>
@@ -3431,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>3</v>
@@ -3470,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>4</v>
@@ -3509,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
         <v>6</v>
@@ -3548,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
         <v>9</v>
@@ -3587,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>19</v>
@@ -3626,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
         <v>36</v>
@@ -3665,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>116</v>
       </c>
@@ -3685,7 +3651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -3725,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>16</v>
@@ -3763,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
         <v>17</v>
@@ -3801,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
         <v>18</v>
@@ -3839,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>3</v>
@@ -3878,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
         <v>4</v>
@@ -3917,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
         <v>6</v>
@@ -3956,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>9</v>
@@ -3995,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
         <v>19</v>
@@ -4034,7 +4000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
         <v>36</v>
@@ -4073,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>116</v>
       </c>
@@ -4089,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>21</v>
       </c>
@@ -4131,7 +4097,7 @@
         <v>-610.1690000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
         <v>35</v>
@@ -4171,7 +4137,7 @@
         <v>-276.4905</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
         <v>38</v>
@@ -4205,11 +4171,11 @@
         <v>0.5</v>
       </c>
       <c r="M68">
-        <f t="shared" ref="M68:M76" si="17">IF(D68,L68*D68*I68,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="M68:M72" si="17">IF(D68,L68*D68*I68,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>116</v>
       </c>
@@ -4225,7 +4191,7 @@
         <v>-278.61850136239781</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>23</v>
       </c>
@@ -4267,7 +4233,7 @@
         <v>-610.1690000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
         <v>35</v>
@@ -4307,7 +4273,7 @@
         <v>-276.4905</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
         <v>38</v>
@@ -4345,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>116</v>
       </c>
@@ -4364,7 +4330,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>27</v>
       </c>
@@ -4375,7 +4341,7 @@
         <v>75</v>
       </c>
       <c r="D74" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -4386,7 +4352,7 @@
       </c>
       <c r="G74">
         <f>IF(D74,F74*D74,0)</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H74">
         <v>-249.58</v>
@@ -4396,21 +4362,21 @@
       </c>
       <c r="J74">
         <f>IF(D74,H74*G74,"")</f>
-        <v>-62.395000000000003</v>
+        <v>-124.79</v>
       </c>
       <c r="L74">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M74">
         <f>IF(D74,L74*D74*I74,0)</f>
         <v>-142.91499999999999</v>
       </c>
       <c r="O74">
-        <f>D74*(I74-H74)</f>
+        <f>G74*(I74-H74)</f>
         <v>-18.124999999999986</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2" t="s">
         <v>26</v>
@@ -4443,18 +4409,18 @@
         <v>0</v>
       </c>
       <c r="L75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M75">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="M75:M76" si="21">IF(D75,L75*D75*I75,0)</f>
         <v>0</v>
       </c>
       <c r="O75">
-        <f t="shared" ref="O75:O76" si="21">D75*(I75-H75)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="O75:O76" si="22">G75*(I75-H75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
         <v>28</v>
@@ -4463,7 +4429,7 @@
         <v>75</v>
       </c>
       <c r="D76" s="10">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -4474,7 +4440,7 @@
       </c>
       <c r="G76">
         <f t="shared" si="20"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="H76">
         <v>-287.2</v>
@@ -4484,27 +4450,27 @@
       </c>
       <c r="J76">
         <f>IF(D76,H76*G76,0)</f>
-        <v>-215.39999999999998</v>
+        <v>-430.79999999999995</v>
       </c>
       <c r="L76">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-428.745</v>
       </c>
       <c r="O76">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2.0550000000000068</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G77">
         <f>SUM(G74:G76)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J77">
         <f>IF(G77=0,0,SUM(J74:J76)/G77)</f>
@@ -4519,12 +4485,12 @@
         <v>-16.069999999999979</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G78">
-        <f>G21+G32+G43+G54+G65+G69+G73+SUM(D74:D76)</f>
+        <f>G21+G32+G43+G54+G65+G69+G73+G77</f>
         <v>9</v>
       </c>
     </row>
@@ -4556,11 +4522,11 @@
   <sheetPr published="0"/>
   <dimension ref="A2:L84"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:B57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -6110,7 +6076,7 @@
         <v>84</v>
       </c>
       <c r="B45">
-        <f>input!D74</f>
+        <f>input!G74</f>
         <v>0.5</v>
       </c>
       <c r="C45">
@@ -6155,7 +6121,7 @@
         <v>86</v>
       </c>
       <c r="B46">
-        <f>input!D75</f>
+        <f>input!G75</f>
         <v>0</v>
       </c>
       <c r="C46">
@@ -6200,7 +6166,7 @@
         <v>85</v>
       </c>
       <c r="B47">
-        <f>input!D76</f>
+        <f>input!G76</f>
         <v>1.5</v>
       </c>
       <c r="C47">
@@ -7617,17 +7583,17 @@
       <selection activeCell="T142" sqref="T142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -7686,7 +7652,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7745,7 +7711,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -7804,7 +7770,7 @@
         <v>-71.22</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -7863,7 +7829,7 @@
         <v>544.22</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -7922,7 +7888,7 @@
         <v>70.569999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -7981,7 +7947,7 @@
         <v>15.35</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -8040,7 +8006,7 @@
         <v>14.24</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -8099,7 +8065,7 @@
         <v>-189.17</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -8158,7 +8124,7 @@
         <v>-256.22000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -8217,7 +8183,7 @@
         <v>-208.92</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -8276,7 +8242,7 @@
         <v>-215.73</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -8335,7 +8301,7 @@
         <v>-212.38</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -8394,7 +8360,7 @@
         <v>-222.87</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -8453,7 +8419,7 @@
         <v>-310</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -8512,7 +8478,7 @@
         <v>-232.84</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -8571,7 +8537,7 @@
         <v>522.89</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -8630,7 +8596,7 @@
         <v>-147.25</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -8689,7 +8655,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>39</v>
@@ -8746,7 +8712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>453</v>
@@ -8803,7 +8769,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>453</v>
@@ -8860,7 +8826,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>453</v>
@@ -8917,7 +8883,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>453</v>
@@ -8974,7 +8940,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>453</v>
@@ -9031,7 +8997,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>453</v>
@@ -9088,7 +9054,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>453</v>
@@ -9145,7 +9111,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>453</v>
@@ -9202,7 +9168,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>453</v>
@@ -9259,7 +9225,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>453</v>
@@ -9316,7 +9282,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <v>453</v>
@@ -9373,7 +9339,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <v>453</v>
@@ -9430,7 +9396,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <v>453</v>
@@ -9487,7 +9453,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <v>453</v>
@@ -9544,7 +9510,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <v>453</v>
@@ -9601,7 +9567,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <v>453</v>
@@ -9658,7 +9624,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <v>453</v>
@@ -9715,7 +9681,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <v>453</v>
@@ -9772,7 +9738,7 @@
         <v>171.85</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>39</v>
@@ -9829,7 +9795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -9906,7 +9872,7 @@
         <v>281.14999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -9983,7 +9949,7 @@
         <v>88.15</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
@@ -10060,7 +10026,7 @@
         <v>243.07</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -10137,7 +10103,7 @@
         <v>372.37</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
@@ -10214,7 +10180,7 @@
         <v>101.28</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
@@ -10291,7 +10257,7 @@
         <v>156.5</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -10368,7 +10334,7 @@
         <v>157.60999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -10445,7 +10411,7 @@
         <v>361.02</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
@@ -10522,7 +10488,7 @@
         <v>428.07000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -10599,7 +10565,7 @@
         <v>380.77</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -10676,7 +10642,7 @@
         <v>387.58</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
@@ -10753,7 +10719,7 @@
         <v>384.23</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
@@ -10830,7 +10796,7 @@
         <v>394.72</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
@@ -10907,7 +10873,7 @@
         <v>481.85</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
@@ -10984,7 +10950,7 @@
         <v>404.69</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
@@ -11061,7 +11027,7 @@
         <v>351.03999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>13</v>
       </c>
@@ -11138,7 +11104,7 @@
         <v>319.10000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
@@ -11215,7 +11181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -11236,12 +11202,12 @@
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>39</v>
       </c>
@@ -11318,7 +11284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -11395,7 +11361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>34</v>
       </c>
@@ -11472,7 +11438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>33</v>
       </c>
@@ -11549,7 +11515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>1</v>
       </c>
@@ -11626,7 +11592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>2</v>
       </c>
@@ -11703,7 +11669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -11780,7 +11746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -11857,7 +11823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -11934,7 +11900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>6</v>
       </c>
@@ -12011,7 +11977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -12088,7 +12054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
@@ -12165,7 +12131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
@@ -12242,7 +12208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>10</v>
       </c>
@@ -12319,7 +12285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -12396,7 +12362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>12</v>
       </c>
@@ -12473,7 +12439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>13</v>
       </c>
@@ -12550,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>14</v>
       </c>
@@ -12627,7 +12593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>39</v>
       </c>
@@ -12683,7 +12649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B82" s="4">
         <f t="array" ref="B82:S99">TRANSPOSE((B62:S79))</f>
         <v>0</v>
@@ -12740,7 +12706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B83" s="4">
         <v>0</v>
       </c>
@@ -12796,7 +12762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B84" s="4">
         <v>0</v>
       </c>
@@ -12852,7 +12818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B85" s="4">
         <v>0</v>
       </c>
@@ -12908,7 +12874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B86" s="4">
         <v>0</v>
       </c>
@@ -12964,7 +12930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B87" s="4">
         <v>0</v>
       </c>
@@ -13020,7 +12986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B88" s="4">
         <v>0</v>
       </c>
@@ -13076,7 +13042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B89" s="4">
         <v>0</v>
       </c>
@@ -13132,7 +13098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B90" s="4">
         <v>0</v>
       </c>
@@ -13188,7 +13154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B91" s="4">
         <v>0</v>
       </c>
@@ -13244,7 +13210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B92" s="4">
         <v>0</v>
       </c>
@@ -13300,7 +13266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B93" s="4">
         <v>0</v>
       </c>
@@ -13356,7 +13322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B94" s="4">
         <v>0</v>
       </c>
@@ -13412,7 +13378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B95" s="4">
         <v>0</v>
       </c>
@@ -13468,7 +13434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B96" s="4">
         <v>0</v>
       </c>
@@ -13524,7 +13490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B97" s="4">
         <v>0</v>
       </c>
@@ -13580,7 +13546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B98" s="4">
         <v>0</v>
       </c>
@@ -13636,7 +13602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B99" s="4">
         <v>0</v>
       </c>
@@ -13692,7 +13658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
         <v>39</v>
       </c>
@@ -13748,7 +13714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>39</v>
       </c>
@@ -13825,7 +13791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -13902,7 +13868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>34</v>
       </c>
@@ -13979,7 +13945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>33</v>
       </c>
@@ -14056,7 +14022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>1</v>
       </c>
@@ -14133,7 +14099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>2</v>
       </c>
@@ -14210,7 +14176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
@@ -14287,7 +14253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>4</v>
       </c>
@@ -14364,7 +14330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -14441,7 +14407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>6</v>
       </c>
@@ -14518,7 +14484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:19" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -14595,7 +14561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
@@ -14672,7 +14638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>9</v>
       </c>
@@ -14749,7 +14715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>10</v>
       </c>
@@ -14826,7 +14792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>11</v>
       </c>
@@ -14903,7 +14869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
@@ -14980,7 +14946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>13</v>
       </c>
@@ -15057,7 +15023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
@@ -15134,7 +15100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B121" s="1" t="s">
         <v>39</v>
       </c>
@@ -15190,7 +15156,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>39</v>
       </c>
@@ -15271,7 +15237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -15352,7 +15318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>34</v>
       </c>
@@ -15433,7 +15399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>33</v>
       </c>
@@ -15514,7 +15480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>1</v>
       </c>
@@ -15595,7 +15561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>2</v>
       </c>
@@ -15676,7 +15642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>3</v>
       </c>
@@ -15757,7 +15723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>4</v>
       </c>
@@ -15838,7 +15804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -15919,7 +15885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>6</v>
       </c>
@@ -16000,7 +15966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -16081,7 +16047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>8</v>
       </c>
@@ -16162,7 +16128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>9</v>
       </c>
@@ -16243,7 +16209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -16324,7 +16290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -16405,7 +16371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>12</v>
       </c>
@@ -16486,7 +16452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>13</v>
       </c>
@@ -16567,7 +16533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
@@ -16648,13 +16614,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="T140" s="4">
         <f>SUM(T122:T139)/2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="S141" s="4" t="s">
         <v>118</v>
       </c>
@@ -16678,14 +16644,14 @@
       <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -16720,7 +16686,7 @@
         <v>-191.72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -16755,7 +16721,7 @@
         <v>-230.79</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -16790,7 +16756,7 @@
         <v>-251.75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -16825,7 +16791,7 @@
         <v>-290.79000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -16860,7 +16826,7 @@
         <v>-108.79</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -16895,7 +16861,7 @@
         <v>-218.94</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -16930,7 +16896,7 @@
         <v>-208.92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -16965,7 +16931,7 @@
         <v>-242.78</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -17000,7 +16966,7 @@
         <v>-243.61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -17035,7 +17001,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -17067,7 +17033,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14">
         <f t="array" ref="B14:K23">TRANSPOSE(B2:K11)</f>
         <v>-191.72</v>
@@ -17100,7 +17066,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>-191.72</v>
       </c>
@@ -17132,7 +17098,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>-191.72</v>
       </c>
@@ -17164,7 +17130,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>-191.72</v>
       </c>
@@ -17196,7 +17162,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>-191.72</v>
       </c>
@@ -17228,7 +17194,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>-191.72</v>
       </c>
@@ -17260,7 +17226,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>-191.72</v>
       </c>
@@ -17292,7 +17258,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>-191.72</v>
       </c>
@@ -17324,7 +17290,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>-191.72</v>
       </c>
@@ -17356,7 +17322,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>-191.72</v>
       </c>
@@ -17388,7 +17354,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>46</v>
       </c>
@@ -17420,7 +17386,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -17465,7 +17431,7 @@
         <v>99.330000000000013</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -17510,7 +17476,7 @@
         <v>60.260000000000019</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -17555,7 +17521,7 @@
         <v>39.300000000000011</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>95</v>
       </c>
@@ -17600,7 +17566,7 @@
         <v>0.25999999999999091</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -17645,7 +17611,7 @@
         <v>182.26</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -17690,7 +17656,7 @@
         <v>72.110000000000014</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -17735,7 +17701,7 @@
         <v>82.130000000000024</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -17780,7 +17746,7 @@
         <v>48.27000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>113</v>
       </c>
@@ -17825,7 +17791,7 @@
         <v>47.44</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -17870,12 +17836,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -17920,7 +17886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -17965,7 +17931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -18010,7 +17976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -18055,7 +18021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -18100,7 +18066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -18145,7 +18111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -18190,7 +18156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>112</v>
       </c>
@@ -18235,7 +18201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>113</v>
       </c>
@@ -18280,7 +18246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -18325,7 +18291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -18357,7 +18323,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50">
         <f t="array" ref="B50:K59">TRANSPOSE(B38:K47)</f>
         <v>0</v>
@@ -18390,7 +18356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>0</v>
       </c>
@@ -18422,7 +18388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>0</v>
       </c>
@@ -18454,7 +18420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>0</v>
       </c>
@@ -18486,7 +18452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>0</v>
       </c>
@@ -18518,7 +18484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>0</v>
       </c>
@@ -18550,7 +18516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>0</v>
       </c>
@@ -18582,7 +18548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>0</v>
       </c>
@@ -18614,7 +18580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>0</v>
       </c>
@@ -18646,7 +18612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>0</v>
       </c>
@@ -18678,7 +18644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>46</v>
       </c>
@@ -18710,7 +18676,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>46</v>
       </c>
@@ -18755,7 +18721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>94</v>
       </c>
@@ -18800,7 +18766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -18845,7 +18811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>95</v>
       </c>
@@ -18890,7 +18856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>109</v>
       </c>
@@ -18935,7 +18901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>110</v>
       </c>
@@ -18980,7 +18946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>111</v>
       </c>
@@ -19025,7 +18991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -19070,7 +19036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>113</v>
       </c>
@@ -19115,7 +19081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>114</v>
       </c>
@@ -19160,7 +19126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>46</v>
       </c>
@@ -19192,7 +19158,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>46</v>
       </c>
@@ -19241,7 +19207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>94</v>
       </c>
@@ -19290,7 +19256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>49</v>
       </c>
@@ -19339,7 +19305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -19388,7 +19354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>109</v>
       </c>
@@ -19437,7 +19403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>110</v>
       </c>
@@ -19486,7 +19452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>111</v>
       </c>
@@ -19535,7 +19501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>112</v>
       </c>
@@ -19584,7 +19550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>113</v>
       </c>
@@ -19633,7 +19599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>114</v>
       </c>
@@ -19682,13 +19648,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L84">
         <f>SUM(L74:L83)/2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K85" t="s">
         <v>120</v>
       </c>
@@ -19707,18 +19673,18 @@
   <sheetPr published="0"/>
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -19753,7 +19719,7 @@
         <v>-191.72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -19788,7 +19754,7 @@
         <v>-230.79</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -19823,7 +19789,7 @@
         <v>-251.75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -19858,7 +19824,7 @@
         <v>-290.79000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -19893,7 +19859,7 @@
         <v>-108.79</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -19928,7 +19894,7 @@
         <v>-218.94</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -19963,7 +19929,7 @@
         <v>-208.92</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -19998,7 +19964,7 @@
         <v>-242.78</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -20033,7 +19999,7 @@
         <v>-243.61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -20068,7 +20034,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -20100,7 +20066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <f t="array" ref="B14:K23">TRANSPOSE(B2:K11)</f>
         <v>-191.72</v>
@@ -20133,7 +20099,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B15" s="2">
         <v>-191.72</v>
       </c>
@@ -20165,7 +20131,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>-191.72</v>
       </c>
@@ -20197,7 +20163,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>-191.72</v>
       </c>
@@ -20229,7 +20195,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>-191.72</v>
       </c>
@@ -20261,7 +20227,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>-191.72</v>
       </c>
@@ -20293,7 +20259,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>-191.72</v>
       </c>
@@ -20325,7 +20291,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>-191.72</v>
       </c>
@@ -20357,7 +20323,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>-191.72</v>
       </c>
@@ -20389,7 +20355,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>-191.72</v>
       </c>
@@ -20421,7 +20387,7 @@
         <v>-291.05</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
@@ -20453,7 +20419,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -20498,7 +20464,7 @@
         <v>99.330000000000013</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -20543,7 +20509,7 @@
         <v>60.260000000000019</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -20588,7 +20554,7 @@
         <v>39.300000000000011</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -20633,7 +20599,7 @@
         <v>0.25999999999999091</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -20678,7 +20644,7 @@
         <v>182.26</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -20723,7 +20689,7 @@
         <v>72.110000000000014</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -20768,7 +20734,7 @@
         <v>82.130000000000024</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -20813,7 +20779,7 @@
         <v>48.27000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
@@ -20858,7 +20824,7 @@
         <v>47.44</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -20903,12 +20869,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
@@ -20953,7 +20919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
@@ -20998,7 +20964,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
@@ -21043,7 +21009,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -21088,7 +21054,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>3</v>
       </c>
@@ -21133,7 +21099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
@@ -21178,7 +21144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -21223,7 +21189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>9</v>
       </c>
@@ -21268,7 +21234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
@@ -21313,7 +21279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
@@ -21358,7 +21324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>13</v>
       </c>
@@ -21390,7 +21356,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50">
         <f t="array" ref="B50:K59">TRANSPOSE(B38:K47)</f>
         <v>0</v>
@@ -21423,7 +21389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0</v>
       </c>
@@ -21455,7 +21421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0</v>
       </c>
@@ -21487,7 +21453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0</v>
       </c>
@@ -21519,7 +21485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0</v>
       </c>
@@ -21551,7 +21517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0</v>
       </c>
@@ -21583,7 +21549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0</v>
       </c>
@@ -21615,7 +21581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0</v>
       </c>
@@ -21647,7 +21613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0</v>
       </c>
@@ -21679,7 +21645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0</v>
       </c>
@@ -21711,7 +21677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>13</v>
       </c>
@@ -21743,7 +21709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>13</v>
       </c>
@@ -21788,7 +21754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>16</v>
       </c>
@@ -21833,7 +21799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>17</v>
       </c>
@@ -21878,7 +21844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>18</v>
       </c>
@@ -21923,7 +21889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
@@ -21968,7 +21934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>4</v>
       </c>
@@ -22013,7 +21979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>6</v>
       </c>
@@ -22058,7 +22024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>9</v>
       </c>
@@ -22103,7 +22069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>19</v>
       </c>
@@ -22148,7 +22114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>36</v>
       </c>
@@ -22193,7 +22159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>13</v>
       </c>
@@ -22225,7 +22191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>13</v>
       </c>
@@ -22274,7 +22240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>16</v>
       </c>
@@ -22323,7 +22289,7 @@
         <v>41.678208000000019</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>17</v>
       </c>
@@ -22372,7 +22338,7 @@
         <v>15.041664000000008</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>18</v>
       </c>
@@ -22421,7 +22387,7 @@
         <v>35.139456000000017</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>3</v>
       </c>
@@ -22470,7 +22436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -22519,7 +22485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>6</v>
       </c>
@@ -22568,7 +22534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>9</v>
       </c>
@@ -22617,7 +22583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>19</v>
       </c>
@@ -22666,7 +22632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>36</v>
       </c>
@@ -22715,13 +22681,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L84">
         <f>SUM(L74:L83)/2</f>
         <v>45.929664000000017</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K85" t="s">
         <v>119</v>
       </c>
@@ -22744,12 +22710,12 @@
       <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -22757,7 +22723,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -22765,7 +22731,7 @@
         <v>-414.8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -22773,7 +22739,7 @@
         <v>-363.17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -22781,7 +22747,7 @@
         <v>-634.91999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -22789,7 +22755,7 @@
         <v>-601.6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -22797,7 +22763,7 @@
         <v>-272.04000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -22805,7 +22771,7 @@
         <v>-826.23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -22813,7 +22779,7 @@
         <v>-1675.7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -22821,7 +22787,7 @@
         <v>-910.7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -22829,7 +22795,7 @@
         <v>-285.83</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -22840,7 +22806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -22851,7 +22817,7 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -22862,7 +22828,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -22873,7 +22839,7 @@
         <v>-92.1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -22884,7 +22850,7 @@
         <v>-134.6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -22895,7 +22861,7 @@
         <v>-181.58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -22906,7 +22872,7 @@
         <v>-242.43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -22917,7 +22883,7 @@
         <v>-199.63</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -22925,7 +22891,7 @@
         <v>-205</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -22956,20 +22922,20 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -22980,7 +22946,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -22991,7 +22957,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -23002,7 +22968,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -23013,14 +22979,14 @@
         <v>-71.22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>87</v>
@@ -23029,7 +22995,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -23040,7 +23006,7 @@
         <v>-191.72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -23051,7 +23017,7 @@
         <v>-230.79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -23062,7 +23028,7 @@
         <v>-251.75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -23073,14 +23039,14 @@
         <v>-290.79000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>87</v>
@@ -23089,7 +23055,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -23100,7 +23066,7 @@
         <v>-285.33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -23111,7 +23077,7 @@
         <v>-260.45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -23122,14 +23088,14 @@
         <v>-310</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>87</v>
@@ -23138,7 +23104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -23149,7 +23115,7 @@
         <v>-88.98</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -23160,7 +23126,7 @@
         <v>-216.99</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -23171,7 +23137,7 @@
         <v>-229.05</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -23182,12 +23148,12 @@
         <v>-288.99</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -23196,7 +23162,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -23205,14 +23171,14 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
@@ -23221,14 +23187,14 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -23237,19 +23203,19 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
@@ -23258,7 +23224,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>60</v>
       </c>
@@ -23267,7 +23233,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>

</xml_diff>